<commit_message>
input data and initialized project
</commit_message>
<xml_diff>
--- a/Honest Abe ERD.xlsx
+++ b/Honest Abe ERD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin of the Lake\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin of the Lake\workspace\Repos\HonestAbe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82FF0132-6A63-4543-BFAC-97D6F8BABCC5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F63575-47A0-4C5E-9DDE-04F2DA5520D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{3FDA8EFD-F085-46B4-9F1D-FEC83BCF469D}"/>
   </bookViews>
@@ -157,12 +157,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,8 +183,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,15 +503,16 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -524,28 +532,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -574,28 +582,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -624,73 +632,73 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -728,73 +736,73 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>